<commit_message>
change all output of tomcat txt->xml
</commit_message>
<xml_diff>
--- a/mwConfigParser_result_20180606.xlsx
+++ b/mwConfigParser_result_20180606.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="39">
   <si>
     <t>Item</t>
   </si>
@@ -81,27 +81,54 @@
 </t>
   </si>
   <si>
-    <t>/WEB-INF/jsp/401.jsp : 401
-/WEB-INF/jsp/403.jsp : 403
-/WEB-INF/jsp/404.jsp : 404</t>
-  </si>
-  <si>
-    <t>url pattern : /*
-	PUT
-	POST
-	DELETE
-	OPTIONS
-	TRACE</t>
+    <t xml:space="preserve">&lt;error-page&gt;
+&lt;error-code&gt;401&lt;/error-code&gt;
+&lt;location&gt;/WEB-INF/jsp/401.jsp&lt;/location&gt;
+&lt;/error-page&gt;
+&lt;error-page&gt;
+&lt;error-code&gt;403&lt;/error-code&gt;
+&lt;location&gt;/WEB-INF/jsp/403.jsp&lt;/location&gt;
+&lt;/error-page&gt;
+&lt;error-page&gt;
+&lt;error-code&gt;404&lt;/error-code&gt;
+&lt;location&gt;/WEB-INF/jsp/404.jsp&lt;/location&gt;
+&lt;/error-page&gt;
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;security-constraint&gt;
+&lt;display-name&gt;Example Security Constraint - part 1&lt;/display-name&gt;
+&lt;web-resource-collection&gt;
+		&lt;web-resource-name&gt;restricted methods&lt;/web-resource-name&gt; 
+		&lt;url-pattern&gt;/*&lt;/url-pattern&gt;
+		&lt;http-method&gt;PUT&lt;/http-method&gt;
+		&lt;http-method&gt;POST&lt;/http-method&gt;
+		&lt;http-method&gt;DELETE&lt;/http-method&gt;
+		&lt;http-method&gt;OPTIONS&lt;/http-method&gt;
+		&lt;http-method&gt;TRACE&lt;/http-method&gt;
+	&lt;/web-resource-collection&gt;
+&lt;auth-constraint/&gt;
+&lt;/security-constraint&gt;
+&lt;security-constraint&gt;
+&lt;display-name&gt;Example Security Constraint - part 2&lt;/display-name&gt;
+&lt;web-resource-collection&gt;
+         &lt;web-resource-name&gt;Protected Area - Deny methods&lt;/web-resource-name&gt;
+         &lt;!-- Define the context-relative URL(s) to be protected --&gt;
+         &lt;url-pattern&gt;/jsp/security/protected/*&lt;/url-pattern&gt;
+         &lt;http-method-omission&gt;DELETE&lt;/http-method-omission&gt;
+         &lt;http-method-omission&gt;GET&lt;/http-method-omission&gt;
+         &lt;http-method-omission&gt;POST&lt;/http-method-omission&gt;
+         &lt;http-method-omission&gt;PUT&lt;/http-method-omission&gt;
+      &lt;/web-resource-collection&gt;
+&lt;auth-constraint/&gt;
+&lt;/security-constraint&gt;
+</t>
   </si>
   <si>
     <t xml:space="preserve">&lt;Host appBase="webapps" autoDeploy="true" name="localhost" unpackWARs="true"&gt;
 &lt;Valve className="org.apache.catalina.valves.AccessLogValve" directory="logs" pattern="%h %l %u %t &amp;quot;%r&amp;quot; %s %b" prefix="localhost_access_log" suffix=".txt"/&gt;
 &lt;/Host&gt;
 </t>
-  </si>
-  <si>
-    <t>false(context.xml)
-default(not use)(server.xml)</t>
   </si>
   <si>
     <t xml:space="preserve">&lt;Connector connectionTimeout="20000" port="8080" protocol="HTTP/1.1" redirectPort="8443" server="null"/&gt;
@@ -418,10 +445,10 @@
         <v>19</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
@@ -460,10 +487,10 @@
         <v>19</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
@@ -481,10 +508,10 @@
         <v>20</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
@@ -502,7 +529,7 @@
         <v>21</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>19</v>
@@ -523,7 +550,7 @@
         <v>22</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>19</v>
@@ -544,10 +571,10 @@
         <v>23</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
@@ -562,13 +589,13 @@
         <v>8</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
@@ -583,10 +610,10 @@
         <v>9</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>19</v>
@@ -607,7 +634,7 @@
         <v>19</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>19</v>

</xml_diff>